<commit_message>
Added sink growth clustering. Still not perfect but a step #11
</commit_message>
<xml_diff>
--- a/tests/atomicdiffusion/diffusion.xlsx
+++ b/tests/atomicdiffusion/diffusion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-9100" yWindow="-19420" windowWidth="18140" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>x</t>
   </si>
@@ -36,15 +36,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>+----------------+----------------+</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> time           </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> point          </t>
-  </si>
-  <si>
     <t>BUCK</t>
   </si>
   <si>
@@ -58,6 +49,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -100,7 +94,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -130,12 +124,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -150,6 +153,10 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -164,6 +171,10 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C10:F34"/>
+  <dimension ref="C10:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -582,13 +593,13 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="3:6">
@@ -596,16 +607,16 @@
         <f>D15</f>
         <v>100000</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <f>$D$11*(1-ERF(0,$D$13/SQRT(4*$D$10*C18)))</f>
         <v>0.70291676752937937</v>
       </c>
-      <c r="E18" s="1">
-        <v>0.69242599999999999</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="E18" s="2">
+        <v>0.69247899999999996</v>
+      </c>
+      <c r="F18" s="2">
         <f>ABS(E18-D18)/D18*100</f>
-        <v>1.4924622677948722</v>
+        <v>1.4849222570214411</v>
       </c>
     </row>
     <row r="19" spans="3:6">
@@ -613,16 +624,16 @@
         <f>C18+$D$15</f>
         <v>200000</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <f t="shared" ref="D19:D22" si="0">$D$11*(1-ERF(0,$D$13/SQRT(4*$D$10*C19)))</f>
         <v>0.7874059071732602</v>
       </c>
-      <c r="E19" s="1">
-        <v>0.78352200000000005</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="E19" s="2">
+        <v>0.78357010000000005</v>
+      </c>
+      <c r="F19" s="2">
         <f t="shared" ref="F19:F22" si="1">ABS(E19-D19)/D19*100</f>
-        <v>0.49325349706902016</v>
+        <v>0.48714483067957542</v>
       </c>
     </row>
     <row r="20" spans="3:6">
@@ -630,16 +641,16 @@
         <f t="shared" ref="C20:C22" si="2">C19+$D$15</f>
         <v>300000</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>0.82572055815224421</v>
       </c>
-      <c r="E20" s="1">
-        <v>0.82357769999999997</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="E20" s="2">
+        <v>0.82359819999999995</v>
+      </c>
+      <c r="F20" s="2">
         <f t="shared" si="1"/>
-        <v>0.25951372181400234</v>
+        <v>0.25703104171144409</v>
       </c>
     </row>
     <row r="21" spans="3:6">
@@ -647,16 +658,16 @@
         <f t="shared" si="2"/>
         <v>400000</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>0.84876608085468808</v>
       </c>
-      <c r="E21" s="1">
-        <v>0.84736529999999999</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="E21" s="2">
+        <v>0.84737580000000001</v>
+      </c>
+      <c r="F21" s="2">
         <f t="shared" si="1"/>
-        <v>0.16503732727838677</v>
+        <v>0.1638002373148657</v>
       </c>
     </row>
     <row r="22" spans="3:6">
@@ -664,80 +675,37 @@
         <f t="shared" si="2"/>
         <v>500000</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>0.86456892451322154</v>
       </c>
-      <c r="E22" s="1">
-        <v>0.86356279999999996</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="E22" s="2">
+        <v>0.86356900000000003</v>
+      </c>
+      <c r="F22" s="2">
         <f t="shared" si="1"/>
-        <v>0.11637296746329992</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6">
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6">
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6">
-      <c r="C28" t="s">
-        <v>5</v>
+        <v>0.11565584707829905</v>
       </c>
     </row>
     <row r="29" spans="3:6">
-      <c r="D29" s="1">
-        <v>100000</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0.69242599999999999</v>
-      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="3:6">
-      <c r="D30" s="1">
-        <v>200000</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0.78352200000000005</v>
-      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="3:6">
-      <c r="D31" s="1">
-        <v>300000</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0.82357769999999997</v>
-      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="3:6">
-      <c r="D32" s="1">
-        <v>400000</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0.84736529999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="D33" s="1">
-        <v>500000</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0.86356279999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5">
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="4:5">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Cleaned out to old kernels for new model
</commit_message>
<xml_diff>
--- a/tests/atomicdiffusion/diffusion.xlsx
+++ b/tests/atomicdiffusion/diffusion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>x</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>% diff</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>Q</t>
   </si>
 </sst>
 </file>
@@ -50,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -94,8 +100,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -136,9 +150,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -157,6 +171,10 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -175,6 +193,10 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -547,21 +569,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C10:F33"/>
+  <dimension ref="C8:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
+    <row r="8" spans="3:4">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1">
+        <v>30000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>355000</v>
+      </c>
+    </row>
     <row r="10" spans="3:4">
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="1">
-        <f>30000000000000*EXP(-355000/8.31446/1000)</f>
-        <v>8.5937016662607408E-6</v>
+        <f>D8*EXP(-D9/8.31446/1000)</f>
+        <v>8.5937016662607404E-9</v>
       </c>
     </row>
     <row r="11" spans="3:4">
@@ -577,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.5</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="3:4">
@@ -603,89 +641,60 @@
       </c>
     </row>
     <row r="18" spans="3:6">
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <f>D15</f>
         <v>100000</v>
       </c>
       <c r="D18" s="2">
         <f>$D$11*(1-ERF(0,$D$13/SQRT(4*$D$10*C18)))</f>
-        <v>0.70291676752937937</v>
+        <v>0.80939255148116862</v>
       </c>
       <c r="E18" s="2">
-        <v>0.69247899999999996</v>
+        <v>0.80870310000000001</v>
       </c>
       <c r="F18" s="2">
         <f>ABS(E18-D18)/D18*100</f>
-        <v>1.4849222570214411</v>
+        <v>8.5181347407624786E-2</v>
       </c>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <f>C18+$D$15</f>
         <v>200000</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ref="D19:D22" si="0">$D$11*(1-ERF(0,$D$13/SQRT(4*$D$10*C19)))</f>
-        <v>0.7874059071732602</v>
+        <v>0.86456892451322154</v>
       </c>
       <c r="E19" s="2">
-        <v>0.78357010000000005</v>
+        <v>0.86431950000000002</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" ref="F19:F22" si="1">ABS(E19-D19)/D19*100</f>
-        <v>0.48714483067957542</v>
+        <v>2.8849581120666868E-2</v>
       </c>
     </row>
     <row r="20" spans="3:6">
-      <c r="C20" s="1">
-        <f t="shared" ref="C20:C22" si="2">C19+$D$15</f>
-        <v>300000</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="0"/>
-        <v>0.82572055815224421</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.82359819999999995</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.25703104171144409</v>
-      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="1">
-        <f t="shared" si="2"/>
-        <v>400000</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="0"/>
-        <v>0.84876608085468808</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.84737580000000001</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.1638002373148657</v>
-      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="3:6">
-      <c r="C22" s="1">
-        <f t="shared" si="2"/>
-        <v>500000</v>
-      </c>
-      <c r="D22" s="2">
-        <f t="shared" si="0"/>
-        <v>0.86456892451322154</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.86356900000000003</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" si="1"/>
-        <v>0.11565584707829905</v>
-      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="29" spans="3:6">
       <c r="D29" s="1"/>

</xml_diff>